<commit_message>
speed up by comparing g-cost pairs
</commit_message>
<xml_diff>
--- a/code/data.xlsx
+++ b/code/data.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB71CF7-7E29-4A96-9982-F4533C9C3D02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C7B60D-3180-417F-BEFF-EF6D615A968E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manually calculation" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="ProgramResult" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2 (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="ProgramResult" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Manually calculation'!$V$1:$V$85</definedName>
@@ -27,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{55E655D8-4EC4-4C38-9B1C-0001C1F1535D}">
@@ -38,16 +39,16 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 4 stages and 4 segments, random driving condition to test whether this works</t>
@@ -62,16 +63,16 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 12 stages and 12 segments; driving conditions for all segments from stage 4 to stage 8 are bad.</t>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="79">
   <si>
     <t>0-25</t>
   </si>
@@ -446,14 +447,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="28">
@@ -887,7 +888,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1171,17 +1172,17 @@
       <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="12" max="12" width="12.86328125" customWidth="1"/>
-    <col min="21" max="21" width="7.73046875" customWidth="1"/>
-    <col min="22" max="22" width="8.1328125" customWidth="1"/>
-    <col min="23" max="23" width="11.1328125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -1205,7 +1206,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1238,7 +1239,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1289,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1341,7 +1342,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1396,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1447,7 +1448,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1481,7 +1482,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -1531,7 +1532,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1587,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1639,7 +1640,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H11" s="3"/>
       <c r="I11" s="13">
         <v>0</v>
@@ -1676,7 +1677,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1719,7 +1720,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>55</v>
@@ -1760,7 +1761,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>75</v>
@@ -1801,7 +1802,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H15" s="3"/>
       <c r="I15" s="25">
         <v>75</v>
@@ -1838,7 +1839,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H16" s="3"/>
       <c r="I16" s="28">
         <v>75</v>
@@ -1875,7 +1876,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H17" s="3"/>
       <c r="I17" s="31">
         <v>75</v>
@@ -1912,7 +1913,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:27" x14ac:dyDescent="0.25">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1928,7 +1929,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G20" s="3"/>
       <c r="H20" s="7">
         <v>0</v>
@@ -2064,7 +2065,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G21" s="3"/>
       <c r="H21" s="7">
         <v>0</v>
@@ -2135,7 +2136,7 @@
         <v>0.31863437499999991</v>
       </c>
     </row>
-    <row r="22" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G22" s="3"/>
       <c r="H22" s="7">
         <v>0</v>
@@ -2206,7 +2207,7 @@
         <v>0.56973437499999979</v>
       </c>
     </row>
-    <row r="23" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G23" s="3"/>
       <c r="H23" s="10">
         <v>0</v>
@@ -2277,7 +2278,7 @@
         <v>1.0325000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G24" s="3"/>
       <c r="H24" s="10">
         <v>0</v>
@@ -2348,7 +2349,7 @@
         <v>9.7121875000000024E-2</v>
       </c>
     </row>
-    <row r="25" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G25" s="3"/>
       <c r="H25" s="10">
         <v>0</v>
@@ -2419,7 +2420,7 @@
         <v>0.15212187500000002</v>
       </c>
     </row>
-    <row r="26" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G26" s="3"/>
       <c r="H26" s="13">
         <v>0</v>
@@ -2490,7 +2491,7 @@
         <v>3.7750000000000013E-2</v>
       </c>
     </row>
-    <row r="27" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G27" s="3"/>
       <c r="H27" s="13">
         <v>0</v>
@@ -2561,7 +2562,7 @@
         <v>0.23970312500000002</v>
       </c>
     </row>
-    <row r="28" spans="7:27" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="7:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G28" s="3"/>
       <c r="H28" s="13">
         <v>0</v>
@@ -2632,7 +2633,7 @@
         <v>0.33657812500000001</v>
       </c>
     </row>
-    <row r="29" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="29" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G29" s="3"/>
       <c r="H29" s="18">
         <v>55</v>
@@ -2703,7 +2704,7 @@
         <v>0.74649999999999994</v>
       </c>
     </row>
-    <row r="30" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="30" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
       <c r="H30" s="18">
         <v>55</v>
@@ -2774,7 +2775,7 @@
         <v>0.92095312499999993</v>
       </c>
     </row>
-    <row r="31" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="31" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
       <c r="H31" s="18">
         <v>55</v>
@@ -2845,7 +2846,7 @@
         <v>1.0078281250000001</v>
       </c>
     </row>
-    <row r="32" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="32" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G32" s="3"/>
       <c r="H32" s="21">
         <v>55</v>
@@ -2916,7 +2917,7 @@
         <v>0.92267187499999992</v>
       </c>
     </row>
-    <row r="33" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="33" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G33" s="3"/>
       <c r="H33" s="21">
         <v>55</v>
@@ -2987,7 +2988,7 @@
         <v>1.146109375</v>
       </c>
     </row>
-    <row r="34" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="34" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G34" s="3"/>
       <c r="H34" s="21">
         <v>55</v>
@@ -3058,7 +3059,7 @@
         <v>1.250796875</v>
       </c>
     </row>
-    <row r="35" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="35" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G35" s="3"/>
       <c r="H35" s="24">
         <v>55</v>
@@ -3129,7 +3130,7 @@
         <v>1.0101718749999997</v>
       </c>
     </row>
-    <row r="36" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="36" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G36" s="3"/>
       <c r="H36" s="24">
         <v>55</v>
@@ -3200,7 +3201,7 @@
         <v>1.2507968749999998</v>
       </c>
     </row>
-    <row r="37" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="37" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G37" s="3">
         <f>(100-0.5*(H37+I37))/J37</f>
         <v>0.46666666666666667</v>
@@ -3278,7 +3279,7 @@
         <v>1.3328281249999998</v>
       </c>
     </row>
-    <row r="38" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="38" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G38" s="3"/>
       <c r="H38" s="27">
         <v>75</v>
@@ -3349,7 +3350,7 @@
         <v>1.3404999999999996</v>
       </c>
     </row>
-    <row r="39" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="39" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G39" s="3"/>
       <c r="H39" s="27">
         <v>75</v>
@@ -3420,7 +3421,7 @@
         <v>1.5562031249999997</v>
       </c>
     </row>
-    <row r="40" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="40" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G40" s="3"/>
       <c r="H40" s="27">
         <v>75</v>
@@ -3491,7 +3492,7 @@
         <v>1.6580781249999998</v>
       </c>
     </row>
-    <row r="41" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="41" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G41" s="3"/>
       <c r="H41" s="30">
         <v>75</v>
@@ -3562,7 +3563,7 @@
         <v>1.5579218749999997</v>
       </c>
     </row>
-    <row r="42" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="42" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G42" s="3"/>
       <c r="H42" s="30">
         <v>75</v>
@@ -3633,7 +3634,7 @@
         <v>1.8226093749999999</v>
       </c>
     </row>
-    <row r="43" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="43" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G43" s="3">
         <f>(100-0.5*(H43+I43))/J43</f>
         <v>0.46666666666666667</v>
@@ -3712,7 +3713,7 @@
         <v>1.9112031249999997</v>
       </c>
     </row>
-    <row r="44" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="44" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G44" s="3"/>
       <c r="H44" s="33">
         <v>75</v>
@@ -3783,7 +3784,7 @@
         <v>1.6604218749999997</v>
       </c>
     </row>
-    <row r="45" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="45" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G45" s="3">
         <f>(100-0.5*(H45+I45))/J45</f>
         <v>0.45454545454545453</v>
@@ -3862,7 +3863,7 @@
         <v>1.6970468749999998</v>
       </c>
     </row>
-    <row r="46" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="46" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G46" s="3">
         <f>(100-0.5*(H46+I46))/J46</f>
         <v>0.33333333333333331</v>
@@ -3941,7 +3942,7 @@
         <v>1.6970468749999998</v>
       </c>
     </row>
-    <row r="47" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="47" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3989,7 +3990,7 @@
         <v>6.8453125000000004E-2</v>
       </c>
     </row>
-    <row r="48" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="48" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -4037,7 +4038,7 @@
         <v>0.176734375</v>
       </c>
     </row>
-    <row r="49" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="49" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -4085,7 +4086,7 @@
         <v>0.23954687499999999</v>
       </c>
     </row>
-    <row r="50" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="50" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -4133,7 +4134,7 @@
         <v>0.17845312499999999</v>
       </c>
     </row>
-    <row r="51" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="51" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -4181,7 +4182,7 @@
         <v>0.33571875000000001</v>
       </c>
     </row>
-    <row r="52" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="52" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R52" s="33">
         <v>55</v>
       </c>
@@ -4218,7 +4219,7 @@
         <v>0.41634375000000001</v>
       </c>
     </row>
-    <row r="53" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="53" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R53" s="35">
         <v>55</v>
       </c>
@@ -4255,7 +4256,7 @@
         <v>0.24189062500000003</v>
       </c>
     </row>
-    <row r="54" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="54" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R54" s="35">
         <v>55</v>
       </c>
@@ -4292,7 +4293,7 @@
         <v>0.41634375000000001</v>
       </c>
     </row>
-    <row r="55" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="55" spans="7:27" x14ac:dyDescent="0.25">
       <c r="Q55">
         <f>(100-0.5*(R55+S55+T55))/U55</f>
         <v>0.46666666666666667</v>
@@ -4334,7 +4335,7 @@
         <v>0.48032812500000005</v>
       </c>
     </row>
-    <row r="56" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="56" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R56" s="34">
         <v>55</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>0.55293437499999976</v>
       </c>
     </row>
-    <row r="57" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="57" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R57" s="34">
         <v>55</v>
       </c>
@@ -4408,7 +4409,7 @@
         <v>0.74801249999999975</v>
       </c>
     </row>
-    <row r="58" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="58" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R58" s="34">
         <v>55</v>
       </c>
@@ -4445,7 +4446,7 @@
         <v>0.84238749999999973</v>
       </c>
     </row>
-    <row r="59" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="59" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R59" s="40">
         <v>55</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>1.3130687499999993</v>
       </c>
     </row>
-    <row r="60" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="60" spans="7:27" x14ac:dyDescent="0.25">
       <c r="Q60">
         <f>(100-0.5*(R60+S60+T60))/U60</f>
         <v>0.31818181818181818</v>
@@ -4524,7 +4525,7 @@
         <v>1.3381812499999994</v>
       </c>
     </row>
-    <row r="61" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="61" spans="7:27" x14ac:dyDescent="0.25">
       <c r="Q61">
         <f>(100-0.5*(R61+S61+T61))/U61</f>
         <v>0.23333333333333334</v>
@@ -4566,7 +4567,7 @@
         <v>1.3381812499999994</v>
       </c>
     </row>
-    <row r="62" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="62" spans="7:27" x14ac:dyDescent="0.25">
       <c r="R62" s="36">
         <v>55</v>
       </c>
@@ -4603,7 +4604,7 @@
         <v>1.7261687499999994</v>
       </c>
     </row>
-    <row r="63" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="63" spans="7:27" x14ac:dyDescent="0.25">
       <c r="Q63">
         <f>(100-0.5*(R63+S63+T63))/U63</f>
         <v>0.13636363636363635</v>
@@ -4645,7 +4646,7 @@
         <v>1.7379812499999994</v>
       </c>
     </row>
-    <row r="64" spans="7:27" x14ac:dyDescent="0.45">
+    <row r="64" spans="7:27" x14ac:dyDescent="0.25">
       <c r="Q64">
         <f>(100-0.5*(R64+S64+T64))/U64</f>
         <v>0.1</v>
@@ -4687,7 +4688,7 @@
         <v>1.7379812499999994</v>
       </c>
     </row>
-    <row r="65" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="65" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R65" s="51">
         <v>55</v>
       </c>
@@ -4724,7 +4725,7 @@
         <v>0.8657968749999998</v>
       </c>
     </row>
-    <row r="66" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="66" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R66" s="46">
         <v>55</v>
       </c>
@@ -4761,7 +4762,7 @@
         <v>1.0918124999999999</v>
       </c>
     </row>
-    <row r="67" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="67" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R67" s="74">
         <v>55</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>1.1974374999999999</v>
       </c>
     </row>
-    <row r="68" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="68" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R68" s="53">
         <v>55</v>
       </c>
@@ -4835,7 +4836,7 @@
         <v>1.7261687499999996</v>
       </c>
     </row>
-    <row r="69" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="69" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q69">
         <f>(100-0.5*(R69+S69+T69))/U69</f>
         <v>0.13636363636363635</v>
@@ -4877,7 +4878,7 @@
         <v>1.7379812499999996</v>
       </c>
     </row>
-    <row r="70" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="70" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q70">
         <f>(100-0.5*(R70+S70+T70))/U70</f>
         <v>0.1</v>
@@ -4919,7 +4920,7 @@
         <v>1.7852312499999996</v>
       </c>
     </row>
-    <row r="71" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="71" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R71" s="54">
         <v>75</v>
       </c>
@@ -4956,7 +4957,7 @@
         <v>0.115328125</v>
       </c>
     </row>
-    <row r="72" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="72" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R72" s="54">
         <v>75</v>
       </c>
@@ -4993,7 +4994,7 @@
         <v>0.24079687500000002</v>
       </c>
     </row>
-    <row r="73" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="73" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R73" s="54">
         <v>75</v>
       </c>
@@ -5030,7 +5031,7 @@
         <v>0.30985937500000005</v>
       </c>
     </row>
-    <row r="74" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="74" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R74" s="57">
         <v>75</v>
       </c>
@@ -5067,7 +5068,7 @@
         <v>0.24251562500000001</v>
       </c>
     </row>
-    <row r="75" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="75" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R75" s="57">
         <v>75</v>
       </c>
@@ -5104,7 +5105,7 @@
         <v>0.41696875</v>
       </c>
     </row>
-    <row r="76" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="76" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q76">
         <f>(100-0.5*(R76+S76+T76))/U76</f>
         <v>0.46666666666666667</v>
@@ -5146,7 +5147,7 @@
         <v>0.48095312500000004</v>
       </c>
     </row>
-    <row r="77" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="77" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R77" s="51">
         <v>75</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>0.31220312500000003</v>
       </c>
     </row>
-    <row r="78" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="78" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q78">
         <f>(100-0.5*(R78+S78+T78))/U78</f>
         <v>0.45454545454545453</v>
@@ -5224,7 +5225,7 @@
         <v>0.33570312500000005</v>
       </c>
     </row>
-    <row r="79" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="79" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q79">
         <f>(100-0.5*(R79+S79+T79))/U79</f>
         <v>0.33333333333333331</v>
@@ -5265,7 +5266,7 @@
         <v>0.33570312500000005</v>
       </c>
     </row>
-    <row r="80" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="80" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R80" s="58">
         <v>75</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>0.65549687499999976</v>
       </c>
     </row>
-    <row r="81" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="81" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R81" s="58">
         <v>75</v>
       </c>
@@ -5339,7 +5340,7 @@
         <v>0.86776249999999977</v>
       </c>
     </row>
-    <row r="82" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="82" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q82">
         <f>(100-0.5*(R82+S82+T82))/U82</f>
         <v>0.46666666666666667</v>
@@ -5380,7 +5381,7 @@
         <v>0.94205937499999981</v>
       </c>
     </row>
-    <row r="83" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="83" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R83" s="50">
         <v>75</v>
       </c>
@@ -5417,7 +5418,7 @@
         <v>1.4713187499999993</v>
       </c>
     </row>
-    <row r="84" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="84" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q84">
         <f>(100-0.5*(R84+S84+T84))/U84</f>
         <v>0.13636363636363635</v>
@@ -5458,7 +5459,7 @@
         <v>1.4825312499999994</v>
       </c>
     </row>
-    <row r="85" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="85" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q85">
         <f>(100-0.5*(R85+S85+T85))/U85</f>
         <v>0.1</v>
@@ -5499,7 +5500,7 @@
         <v>1.4825312499999994</v>
       </c>
     </row>
-    <row r="86" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="86" spans="17:27" x14ac:dyDescent="0.25">
       <c r="R86" s="61">
         <v>75</v>
       </c>
@@ -5536,7 +5537,7 @@
         <v>0.98860937499999979</v>
       </c>
     </row>
-    <row r="87" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="87" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q87">
         <f>(100-0.5*(R87+S87+T87))/U87</f>
         <v>0.45454545454545453</v>
@@ -5577,7 +5578,7 @@
         <v>1.0196093749999997</v>
       </c>
     </row>
-    <row r="88" spans="17:27" x14ac:dyDescent="0.45">
+    <row r="88" spans="17:27" x14ac:dyDescent="0.25">
       <c r="Q88">
         <f>(100-0.5*(R88+S88+T88))/U88</f>
         <v>0.33333333333333331</v>
@@ -5632,16 +5633,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -5651,7 +5652,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -5709,7 +5710,7 @@
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -5819,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -5929,7 +5930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -5985,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -6039,7 +6040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -6149,7 +6150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -6205,7 +6206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -6259,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -6369,7 +6370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>63</v>
       </c>
@@ -6425,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="90"/>
       <c r="B16" s="90" t="s">
         <v>7</v>
@@ -6479,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
         <v>64</v>
       </c>
@@ -6535,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="90"/>
       <c r="B18" s="90" t="s">
         <v>7</v>
@@ -6589,7 +6590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="90" t="s">
         <v>65</v>
       </c>
@@ -6645,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="90"/>
       <c r="B20" s="90" t="s">
         <v>7</v>
@@ -6699,7 +6700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="90" t="s">
         <v>66</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="90"/>
       <c r="B22" s="90" t="s">
         <v>7</v>
@@ -6809,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
@@ -6865,7 +6866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>7</v>
@@ -6919,7 +6920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -6975,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -7029,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -7085,7 +7086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>7</v>
@@ -7139,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -7195,7 +7196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
@@ -7249,7 +7250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
@@ -7305,7 +7306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>7</v>
@@ -7359,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -7415,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>7</v>
@@ -7476,6 +7477,1113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901D95BA-A164-4B4B-B07A-FB08C567B29D}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="90"/>
+      <c r="B16" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="90"/>
+      <c r="B18" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="90"/>
+      <c r="B20" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="90" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="90"/>
+      <c r="B22" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S35"/>
   <sheetViews>
@@ -7483,14 +8591,14 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" s="87"/>
       <c r="D2" s="87"/>
       <c r="E2" s="87"/>
@@ -7509,7 +8617,7 @@
       <c r="R2" s="87"/>
       <c r="S2" s="86"/>
     </row>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="91" t="s">
         <v>73</v>
       </c>
@@ -7542,7 +8650,7 @@
       <c r="R3" s="87"/>
       <c r="S3" s="86"/>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" s="87"/>
       <c r="D4" s="87">
         <v>1</v>
@@ -7573,7 +8681,7 @@
       <c r="R4" s="87"/>
       <c r="S4" s="86"/>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5" s="87"/>
       <c r="D5" s="87">
         <v>1</v>
@@ -7604,7 +8712,7 @@
       <c r="R5" s="87"/>
       <c r="S5" s="86"/>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6" s="87"/>
       <c r="D6" s="87">
         <v>1</v>
@@ -7635,7 +8743,7 @@
       <c r="R6" s="87"/>
       <c r="S6" s="86"/>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7" s="87"/>
       <c r="D7" s="87">
         <v>1</v>
@@ -7666,7 +8774,7 @@
       <c r="R7" s="87"/>
       <c r="S7" s="86"/>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8" s="87"/>
       <c r="D8" s="87">
         <v>1</v>
@@ -7697,7 +8805,7 @@
       <c r="R8" s="87"/>
       <c r="S8" s="86"/>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" s="87"/>
       <c r="D9" s="87">
         <v>1</v>
@@ -7728,7 +8836,7 @@
       <c r="R9" s="87"/>
       <c r="S9" s="86"/>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10" s="87"/>
       <c r="D10" s="87">
         <v>5</v>
@@ -7759,7 +8867,7 @@
       <c r="R10" s="87"/>
       <c r="S10" s="86"/>
     </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="87"/>
       <c r="D11" s="87">
         <v>10</v>
@@ -7790,7 +8898,7 @@
       <c r="R11" s="87"/>
       <c r="S11" s="86"/>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C12" s="87"/>
       <c r="D12" s="87">
         <v>25</v>
@@ -7821,7 +8929,7 @@
       <c r="R12" s="87"/>
       <c r="S12" s="86"/>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="87"/>
       <c r="D13" s="87">
         <v>50</v>
@@ -7852,7 +8960,7 @@
       <c r="R13" s="87"/>
       <c r="S13" s="86"/>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C14" s="87"/>
       <c r="D14" s="87">
         <v>100</v>
@@ -7883,7 +8991,7 @@
       <c r="R14" s="87"/>
       <c r="S14" s="86"/>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" s="87"/>
       <c r="D15" s="87"/>
       <c r="E15" s="87"/>
@@ -7902,7 +9010,7 @@
       <c r="R15" s="87"/>
       <c r="S15" s="86"/>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="91" t="s">
         <v>74</v>
       </c>
@@ -7935,7 +9043,7 @@
       <c r="R16" s="87"/>
       <c r="S16" s="86"/>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="87"/>
       <c r="D17" s="87">
         <v>1</v>
@@ -7967,7 +9075,7 @@
       <c r="R17" s="87"/>
       <c r="S17" s="86"/>
     </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="87"/>
       <c r="D18" s="87">
         <v>1</v>
@@ -7999,7 +9107,7 @@
       <c r="R18" s="87"/>
       <c r="S18" s="86"/>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="87"/>
       <c r="D19" s="87">
         <v>1</v>
@@ -8017,7 +9125,7 @@
         <v>78</v>
       </c>
       <c r="I19" s="87">
-        <f t="shared" ref="I18:I22" si="0">D19*G19+F19*E19</f>
+        <f t="shared" ref="I19:I22" si="0">D19*G19+F19*E19</f>
         <v>32.563988749999901</v>
       </c>
       <c r="J19" s="87"/>
@@ -8031,7 +9139,7 @@
       <c r="R19" s="87"/>
       <c r="S19" s="86"/>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="87"/>
       <c r="D20" s="87">
         <v>1</v>
@@ -8063,7 +9171,7 @@
       <c r="R20" s="87"/>
       <c r="S20" s="86"/>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="87"/>
       <c r="D21" s="87">
         <v>1</v>
@@ -8095,7 +9203,7 @@
       <c r="R21" s="87"/>
       <c r="S21" s="86"/>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="87"/>
       <c r="D22" s="87">
         <v>1</v>
@@ -8127,7 +9235,7 @@
       <c r="R22" s="87"/>
       <c r="S22" s="86"/>
     </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="87"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
@@ -8146,7 +9254,7 @@
       <c r="R23" s="87"/>
       <c r="S23" s="86"/>
     </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="87"/>
       <c r="D24" s="87"/>
       <c r="E24" s="87"/>
@@ -8165,7 +9273,7 @@
       <c r="R24" s="87"/>
       <c r="S24" s="86"/>
     </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="87"/>
       <c r="D25" s="87"/>
       <c r="E25" s="87"/>
@@ -8184,7 +9292,7 @@
       <c r="R25" s="87"/>
       <c r="S25" s="86"/>
     </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="87"/>
       <c r="D26" s="87"/>
       <c r="E26" s="87"/>
@@ -8203,7 +9311,7 @@
       <c r="R26" s="87"/>
       <c r="S26" s="86"/>
     </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27" s="87"/>
       <c r="D27" s="87"/>
       <c r="E27" s="87"/>
@@ -8222,7 +9330,7 @@
       <c r="R27" s="87"/>
       <c r="S27" s="86"/>
     </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28" s="87"/>
       <c r="D28" s="87"/>
       <c r="E28" s="87"/>
@@ -8241,7 +9349,7 @@
       <c r="R28" s="87"/>
       <c r="S28" s="86"/>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="87"/>
       <c r="D29" s="87"/>
       <c r="E29" s="87"/>
@@ -8260,7 +9368,7 @@
       <c r="R29" s="87"/>
       <c r="S29" s="86"/>
     </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="86"/>
       <c r="D30" s="86"/>
       <c r="E30" s="86"/>
@@ -8279,7 +9387,7 @@
       <c r="R30" s="86"/>
       <c r="S30" s="86"/>
     </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C31" s="86"/>
       <c r="D31" s="86"/>
       <c r="E31" s="86"/>
@@ -8298,7 +9406,7 @@
       <c r="R31" s="86"/>
       <c r="S31" s="86"/>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="86"/>
       <c r="D32" s="86"/>
       <c r="E32" s="86"/>
@@ -8317,7 +9425,7 @@
       <c r="R32" s="86"/>
       <c r="S32" s="86"/>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="86"/>
       <c r="D33" s="86"/>
       <c r="E33" s="86"/>
@@ -8336,7 +9444,7 @@
       <c r="R33" s="86"/>
       <c r="S33" s="86"/>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" s="86"/>
       <c r="D34" s="86"/>
       <c r="E34" s="86"/>
@@ -8355,7 +9463,7 @@
       <c r="R34" s="86"/>
       <c r="S34" s="86"/>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35" s="86"/>
       <c r="D35" s="86"/>
       <c r="E35" s="86"/>

</xml_diff>